<commit_message>
data_fetch updates plus+notes in excel
</commit_message>
<xml_diff>
--- a/Worrell Lab Sample Data/3-12-24 Zac Sample Fluoresence Data.xlsx
+++ b/Worrell Lab Sample Data/3-12-24 Zac Sample Fluoresence Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oppos\Desktop\worrell-pr\Worrell Lab Sample Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6898069C-D7AB-4075-9B49-E1E10B1E1793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933132BF-84F9-44D4-AA38-AE3930952C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C63595E6-F245-4A81-A66B-C051BF7F32E4}"/>
+    <workbookView xWindow="24" yWindow="12" windowWidth="23016" windowHeight="12348" xr2:uid="{C63595E6-F245-4A81-A66B-C051BF7F32E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet7" sheetId="9" r:id="rId1"/>
@@ -55,7 +55,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Tecan.At.Common, 3.9.1.0
 Tecan.At.Common.DocumentManagement, 3.9.1.0
@@ -120,7 +120,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
 MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
@@ -150,7 +150,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Tecan.At.Common, 3.9.1.0
 Tecan.At.Common.DocumentManagement, 3.9.1.0
@@ -215,7 +215,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
 MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
@@ -245,7 +245,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Tecan.At.Common, 3.9.1.0
 Tecan.At.Common.DocumentManagement, 3.9.1.0
@@ -310,7 +310,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
 MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
@@ -340,7 +340,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Tecan.At.Common, 3.9.1.0
 Tecan.At.Common.DocumentManagement, 3.9.1.0
@@ -405,7 +405,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
 MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
@@ -435,7 +435,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Tecan.At.Common, 3.9.1.0
 Tecan.At.Common.DocumentManagement, 3.9.1.0
@@ -500,7 +500,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
 MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
@@ -530,7 +530,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Tecan.At.Common, 3.9.1.0
 Tecan.At.Common.DocumentManagement, 3.9.1.0
@@ -595,7 +595,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
 MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
@@ -612,7 +612,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="197">
   <si>
     <t>Application: Tecan i-control</t>
   </si>
@@ -1185,6 +1185,24 @@
   </si>
   <si>
     <t>Sheet One</t>
+  </si>
+  <si>
+    <t>molecular weight vs fluor readout (1) ---temperature vs fluor readout</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>1st deriv?</t>
+  </si>
+  <si>
+    <t>individual well</t>
   </si>
 </sst>
 </file>
@@ -1218,10 +1236,10 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1276,6 +1294,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1296,12 +1320,19 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2768,13 +2799,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C2F53B6-9B06-4BF7-93D9-D918FFE784F6}">
   <dimension ref="A1:S153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A153" sqref="A153"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2782,7 +2813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2790,7 +2821,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2798,7 +2829,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2806,7 +2837,7 @@
         <v>45363</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2814,7 +2845,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2822,7 +2853,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -2830,7 +2861,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -2838,17 +2869,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -2856,7 +2887,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -2864,7 +2895,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -2875,7 +2906,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -2886,7 +2917,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -2897,7 +2928,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -2908,7 +2939,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -2919,7 +2950,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -2930,7 +2961,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -2938,7 +2969,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -2949,7 +2980,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -2960,7 +2991,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -2971,7 +3002,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -2982,7 +3013,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -2993,7 +3024,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -3001,12 +3032,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>65</v>
       </c>
@@ -3065,7 +3096,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>66</v>
       </c>
@@ -3124,7 +3155,7 @@
         <v>4652</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>67</v>
       </c>
@@ -3183,7 +3214,7 @@
         <v>26655</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>68</v>
       </c>
@@ -3242,7 +3273,7 @@
         <v>44395</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>69</v>
       </c>
@@ -3301,7 +3332,7 @@
         <v>54411</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>70</v>
       </c>
@@ -3360,7 +3391,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>71</v>
       </c>
@@ -3419,7 +3450,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>72</v>
       </c>
@@ -3478,7 +3509,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>73</v>
       </c>
@@ -3537,7 +3568,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>74</v>
       </c>
@@ -3596,7 +3627,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>75</v>
       </c>
@@ -3655,7 +3686,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>76</v>
       </c>
@@ -3714,7 +3745,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>77</v>
       </c>
@@ -3773,7 +3804,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>78</v>
       </c>
@@ -3832,7 +3863,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>79</v>
       </c>
@@ -3891,7 +3922,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>80</v>
       </c>
@@ -3950,7 +3981,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>81</v>
       </c>
@@ -4009,7 +4040,7 @@
         <v>6622</v>
       </c>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>82</v>
       </c>
@@ -4068,7 +4099,7 @@
         <v>29281</v>
       </c>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>83</v>
       </c>
@@ -4127,7 +4158,7 @@
         <v>15789</v>
       </c>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>84</v>
       </c>
@@ -4186,7 +4217,7 @@
         <v>45418</v>
       </c>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>85</v>
       </c>
@@ -4245,7 +4276,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>86</v>
       </c>
@@ -4304,7 +4335,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>87</v>
       </c>
@@ -4363,7 +4394,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>88</v>
       </c>
@@ -4422,7 +4453,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
         <v>89</v>
       </c>
@@ -4481,7 +4512,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>90</v>
       </c>
@@ -4540,7 +4571,7 @@
         <v>25801</v>
       </c>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>91</v>
       </c>
@@ -4599,7 +4630,7 @@
         <v>17403</v>
       </c>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>92</v>
       </c>
@@ -4658,7 +4689,7 @@
         <v>38026</v>
       </c>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>93</v>
       </c>
@@ -4717,7 +4748,7 @@
         <v>18766</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>94</v>
       </c>
@@ -4776,7 +4807,7 @@
         <v>18948</v>
       </c>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>95</v>
       </c>
@@ -4835,7 +4866,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>96</v>
       </c>
@@ -4894,7 +4925,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>97</v>
       </c>
@@ -4953,7 +4984,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>98</v>
       </c>
@@ -5012,7 +5043,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
         <v>99</v>
       </c>
@@ -5071,7 +5102,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>100</v>
       </c>
@@ -5130,7 +5161,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
         <v>101</v>
       </c>
@@ -5189,7 +5220,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>102</v>
       </c>
@@ -5248,7 +5279,7 @@
         <v>18909</v>
       </c>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>103</v>
       </c>
@@ -5307,7 +5338,7 @@
         <v>7334</v>
       </c>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>104</v>
       </c>
@@ -5366,7 +5397,7 @@
         <v>9265</v>
       </c>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>105</v>
       </c>
@@ -5425,7 +5456,7 @@
         <v>37072</v>
       </c>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
         <v>106</v>
       </c>
@@ -5484,7 +5515,7 @@
         <v>12443</v>
       </c>
     </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
         <v>107</v>
       </c>
@@ -5543,7 +5574,7 @@
         <v>14268</v>
       </c>
     </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
         <v>108</v>
       </c>
@@ -5602,7 +5633,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
         <v>109</v>
       </c>
@@ -5661,7 +5692,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
         <v>110</v>
       </c>
@@ -5720,7 +5751,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
         <v>111</v>
       </c>
@@ -5779,7 +5810,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
         <v>112</v>
       </c>
@@ -5838,7 +5869,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
         <v>113</v>
       </c>
@@ -5897,7 +5928,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
         <v>114</v>
       </c>
@@ -5956,7 +5987,7 @@
         <v>11958</v>
       </c>
     </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
         <v>115</v>
       </c>
@@ -6015,7 +6046,7 @@
         <v>11811</v>
       </c>
     </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
         <v>116</v>
       </c>
@@ -6074,7 +6105,7 @@
         <v>13066</v>
       </c>
     </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
         <v>117</v>
       </c>
@@ -6133,7 +6164,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
         <v>118</v>
       </c>
@@ -6192,7 +6223,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
         <v>119</v>
       </c>
@@ -6251,7 +6282,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
         <v>120</v>
       </c>
@@ -6310,7 +6341,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
         <v>121</v>
       </c>
@@ -6369,7 +6400,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
         <v>122</v>
       </c>
@@ -6428,7 +6459,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
         <v>123</v>
       </c>
@@ -6487,7 +6518,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
         <v>124</v>
       </c>
@@ -6546,7 +6577,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
         <v>125</v>
       </c>
@@ -6605,7 +6636,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
         <v>126</v>
       </c>
@@ -6664,7 +6695,7 @@
         <v>14257</v>
       </c>
     </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="s">
         <v>127</v>
       </c>
@@ -6723,7 +6754,7 @@
         <v>15741</v>
       </c>
     </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="s">
         <v>128</v>
       </c>
@@ -6782,7 +6813,7 @@
         <v>19461</v>
       </c>
     </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
         <v>129</v>
       </c>
@@ -6841,7 +6872,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
         <v>130</v>
       </c>
@@ -6900,7 +6931,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
         <v>131</v>
       </c>
@@ -6959,7 +6990,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
         <v>132</v>
       </c>
@@ -7018,7 +7049,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
         <v>133</v>
       </c>
@@ -7077,7 +7108,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
         <v>134</v>
       </c>
@@ -7136,7 +7167,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
         <v>135</v>
       </c>
@@ -7195,7 +7226,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
         <v>136</v>
       </c>
@@ -7254,7 +7285,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
         <v>137</v>
       </c>
@@ -7313,7 +7344,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
         <v>138</v>
       </c>
@@ -7372,7 +7403,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="s">
         <v>139</v>
       </c>
@@ -7431,7 +7462,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="s">
         <v>140</v>
       </c>
@@ -7490,7 +7521,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="s">
         <v>141</v>
       </c>
@@ -7549,7 +7580,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
         <v>142</v>
       </c>
@@ -7608,7 +7639,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="s">
         <v>143</v>
       </c>
@@ -7667,7 +7698,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
         <v>144</v>
       </c>
@@ -7726,7 +7757,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
         <v>145</v>
       </c>
@@ -7785,7 +7816,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="s">
         <v>146</v>
       </c>
@@ -7844,7 +7875,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="s">
         <v>147</v>
       </c>
@@ -7903,7 +7934,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
         <v>148</v>
       </c>
@@ -7962,7 +7993,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="s">
         <v>149</v>
       </c>
@@ -8021,7 +8052,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="s">
         <v>150</v>
       </c>
@@ -8080,7 +8111,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A138" s="3" t="s">
         <v>151</v>
       </c>
@@ -8139,7 +8170,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="s">
         <v>152</v>
       </c>
@@ -8198,7 +8229,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="s">
         <v>153</v>
       </c>
@@ -8257,7 +8288,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="141" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="s">
         <v>154</v>
       </c>
@@ -8316,7 +8347,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="142" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="s">
         <v>155</v>
       </c>
@@ -8375,7 +8406,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="143" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="s">
         <v>156</v>
       </c>
@@ -8434,7 +8465,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="144" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="s">
         <v>157</v>
       </c>
@@ -8493,7 +8524,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="145" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A145" s="3" t="s">
         <v>158</v>
       </c>
@@ -8552,7 +8583,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="146" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A146" s="3" t="s">
         <v>159</v>
       </c>
@@ -8611,7 +8642,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="147" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A147" s="3" t="s">
         <v>160</v>
       </c>
@@ -8670,7 +8701,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="148" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A148" s="3" t="s">
         <v>161</v>
       </c>
@@ -8729,7 +8760,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="153" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>48</v>
       </c>
@@ -8748,13 +8779,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FD080A5-183B-41D0-94A3-9546A692E84F}">
   <dimension ref="A1:S153"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8762,7 +8793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -8770,7 +8801,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -8778,7 +8809,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -8786,7 +8817,7 @@
         <v>45363</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -8794,7 +8825,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -8802,7 +8833,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -8810,7 +8841,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -8818,17 +8849,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -8836,144 +8867,185 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E17" t="s">
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E18">
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6">
         <v>750</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E19">
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6">
         <v>375</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E20">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6">
         <v>480</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E21">
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6">
         <v>5</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E22">
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6">
         <v>5</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E23">
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8">
         <v>150</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E24">
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6">
         <v>50</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E25">
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6">
         <v>400</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E26">
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6">
         <v>20</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E27">
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6">
         <v>0</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E28">
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6">
         <v>10</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E29">
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6">
         <v>20000</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -8981,19 +9053,68 @@
         <v>183</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I43" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="7"/>
+    </row>
+    <row r="44" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="7"/>
+    </row>
+    <row r="45" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="7"/>
+    </row>
+    <row r="46" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I46" s="7"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="7"/>
+      <c r="L46" s="7"/>
+    </row>
+    <row r="47" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="7"/>
+      <c r="N47" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="I49" t="s">
+        <v>192</v>
+      </c>
+      <c r="J49" t="s">
+        <v>193</v>
+      </c>
+      <c r="K49" t="s">
+        <v>194</v>
+      </c>
+      <c r="M49" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" s="9" t="s">
         <v>163</v>
       </c>
       <c r="D52" s="3" t="s">
@@ -9045,14 +9166,14 @@
         <v>179</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="6">
         <v>4308</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="8">
         <v>465</v>
       </c>
       <c r="D53">
@@ -9104,7 +9225,7 @@
         <v>4686</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>67</v>
       </c>
@@ -9163,7 +9284,7 @@
         <v>26990</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>68</v>
       </c>
@@ -9222,7 +9343,7 @@
         <v>44695</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>69</v>
       </c>
@@ -9281,7 +9402,7 @@
         <v>55003</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>70</v>
       </c>
@@ -9340,7 +9461,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>71</v>
       </c>
@@ -9399,7 +9520,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>72</v>
       </c>
@@ -9458,7 +9579,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>73</v>
       </c>
@@ -9517,7 +9638,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>74</v>
       </c>
@@ -9576,7 +9697,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>75</v>
       </c>
@@ -9635,7 +9756,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>76</v>
       </c>
@@ -9694,7 +9815,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>77</v>
       </c>
@@ -9753,7 +9874,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>78</v>
       </c>
@@ -9812,7 +9933,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>79</v>
       </c>
@@ -9871,7 +9992,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>80</v>
       </c>
@@ -9930,7 +10051,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>81</v>
       </c>
@@ -9989,7 +10110,7 @@
         <v>6629</v>
       </c>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>82</v>
       </c>
@@ -10048,7 +10169,7 @@
         <v>29666</v>
       </c>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>83</v>
       </c>
@@ -10107,7 +10228,7 @@
         <v>16149</v>
       </c>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>84</v>
       </c>
@@ -10166,7 +10287,7 @@
         <v>46597</v>
       </c>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>85</v>
       </c>
@@ -10225,7 +10346,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>86</v>
       </c>
@@ -10284,7 +10405,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>87</v>
       </c>
@@ -10343,7 +10464,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>88</v>
       </c>
@@ -10402,7 +10523,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
         <v>89</v>
       </c>
@@ -10461,7 +10582,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>90</v>
       </c>
@@ -10520,7 +10641,7 @@
         <v>26465</v>
       </c>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>91</v>
       </c>
@@ -10579,7 +10700,7 @@
         <v>17598</v>
       </c>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>92</v>
       </c>
@@ -10638,7 +10759,7 @@
         <v>38089</v>
       </c>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>93</v>
       </c>
@@ -10697,7 +10818,7 @@
         <v>18996</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>94</v>
       </c>
@@ -10756,7 +10877,7 @@
         <v>19106</v>
       </c>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>95</v>
       </c>
@@ -10815,7 +10936,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>96</v>
       </c>
@@ -10874,7 +10995,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>97</v>
       </c>
@@ -10933,7 +11054,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>98</v>
       </c>
@@ -10992,7 +11113,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
         <v>99</v>
       </c>
@@ -11051,7 +11172,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>100</v>
       </c>
@@ -11110,7 +11231,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
         <v>101</v>
       </c>
@@ -11169,7 +11290,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>102</v>
       </c>
@@ -11228,7 +11349,7 @@
         <v>18882</v>
       </c>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>103</v>
       </c>
@@ -11287,7 +11408,7 @@
         <v>7312</v>
       </c>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>104</v>
       </c>
@@ -11346,7 +11467,7 @@
         <v>9290</v>
       </c>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>105</v>
       </c>
@@ -11405,7 +11526,7 @@
         <v>37216</v>
       </c>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
         <v>106</v>
       </c>
@@ -11464,7 +11585,7 @@
         <v>12530</v>
       </c>
     </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
         <v>107</v>
       </c>
@@ -11523,7 +11644,7 @@
         <v>14347</v>
       </c>
     </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
         <v>108</v>
       </c>
@@ -11582,7 +11703,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
         <v>109</v>
       </c>
@@ -11641,7 +11762,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
         <v>110</v>
       </c>
@@ -11700,7 +11821,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
         <v>111</v>
       </c>
@@ -11759,7 +11880,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
         <v>112</v>
       </c>
@@ -11818,7 +11939,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
         <v>113</v>
       </c>
@@ -11877,7 +11998,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
         <v>114</v>
       </c>
@@ -11936,7 +12057,7 @@
         <v>12137</v>
       </c>
     </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
         <v>115</v>
       </c>
@@ -11995,7 +12116,7 @@
         <v>11966</v>
       </c>
     </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
         <v>116</v>
       </c>
@@ -12054,7 +12175,7 @@
         <v>13289</v>
       </c>
     </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
         <v>117</v>
       </c>
@@ -12113,7 +12234,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
         <v>118</v>
       </c>
@@ -12172,7 +12293,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
         <v>119</v>
       </c>
@@ -12231,7 +12352,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
         <v>120</v>
       </c>
@@ -12290,7 +12411,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
         <v>121</v>
       </c>
@@ -12349,7 +12470,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
         <v>122</v>
       </c>
@@ -12408,7 +12529,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
         <v>123</v>
       </c>
@@ -12467,7 +12588,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
         <v>124</v>
       </c>
@@ -12526,7 +12647,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
         <v>125</v>
       </c>
@@ -12585,7 +12706,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
         <v>126</v>
       </c>
@@ -12644,7 +12765,7 @@
         <v>14312</v>
       </c>
     </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="s">
         <v>127</v>
       </c>
@@ -12703,7 +12824,7 @@
         <v>16002</v>
       </c>
     </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="s">
         <v>128</v>
       </c>
@@ -12762,7 +12883,7 @@
         <v>19728</v>
       </c>
     </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
         <v>129</v>
       </c>
@@ -12821,7 +12942,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
         <v>130</v>
       </c>
@@ -12880,7 +13001,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
         <v>131</v>
       </c>
@@ -12939,7 +13060,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
         <v>132</v>
       </c>
@@ -12998,7 +13119,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
         <v>133</v>
       </c>
@@ -13057,7 +13178,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
         <v>134</v>
       </c>
@@ -13116,7 +13237,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
         <v>135</v>
       </c>
@@ -13175,7 +13296,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
         <v>136</v>
       </c>
@@ -13234,7 +13355,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
         <v>137</v>
       </c>
@@ -13293,7 +13414,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
         <v>138</v>
       </c>
@@ -13352,7 +13473,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="s">
         <v>139</v>
       </c>
@@ -13411,7 +13532,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="s">
         <v>140</v>
       </c>
@@ -13470,7 +13591,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="s">
         <v>141</v>
       </c>
@@ -13529,7 +13650,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
         <v>142</v>
       </c>
@@ -13588,7 +13709,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="s">
         <v>143</v>
       </c>
@@ -13647,7 +13768,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
         <v>144</v>
       </c>
@@ -13706,7 +13827,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
         <v>145</v>
       </c>
@@ -13765,7 +13886,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="s">
         <v>146</v>
       </c>
@@ -13824,7 +13945,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="s">
         <v>147</v>
       </c>
@@ -13883,7 +14004,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
         <v>148</v>
       </c>
@@ -13942,7 +14063,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="s">
         <v>149</v>
       </c>
@@ -14001,7 +14122,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="s">
         <v>150</v>
       </c>
@@ -14060,7 +14181,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A138" s="3" t="s">
         <v>151</v>
       </c>
@@ -14119,7 +14240,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="s">
         <v>152</v>
       </c>
@@ -14178,7 +14299,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="s">
         <v>153</v>
       </c>
@@ -14237,7 +14358,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="141" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="s">
         <v>154</v>
       </c>
@@ -14296,7 +14417,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="142" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="s">
         <v>155</v>
       </c>
@@ -14355,7 +14476,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="143" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="s">
         <v>156</v>
       </c>
@@ -14414,7 +14535,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="144" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="s">
         <v>157</v>
       </c>
@@ -14473,7 +14594,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="145" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A145" s="3" t="s">
         <v>158</v>
       </c>
@@ -14532,7 +14653,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="146" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A146" s="3" t="s">
         <v>159</v>
       </c>
@@ -14591,7 +14712,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="147" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A147" s="3" t="s">
         <v>160</v>
       </c>
@@ -14650,7 +14771,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="148" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A148" s="3" t="s">
         <v>161</v>
       </c>
@@ -14709,7 +14830,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="153" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>48</v>
       </c>
@@ -14718,6 +14839,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I43:L47"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -14730,9 +14854,9 @@
   <sheetViews>
     <sheetView topLeftCell="A46" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -14740,7 +14864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -14748,7 +14872,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -14756,7 +14880,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -14764,7 +14888,7 @@
         <v>45363</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -14772,7 +14896,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -14780,7 +14904,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -14788,7 +14912,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -14796,17 +14920,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -14814,7 +14938,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -14822,7 +14946,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -14833,7 +14957,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -14844,7 +14968,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -14855,7 +14979,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -14866,7 +14990,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -14877,7 +15001,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -14888,7 +15012,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -14896,7 +15020,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -14907,7 +15031,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -14918,7 +15042,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -14929,7 +15053,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -14940,7 +15064,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -14951,7 +15075,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -14959,12 +15083,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>65</v>
       </c>
@@ -15023,7 +15147,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>66</v>
       </c>
@@ -15082,7 +15206,7 @@
         <v>43387</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>67</v>
       </c>
@@ -15141,7 +15265,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>68</v>
       </c>
@@ -15200,7 +15324,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>69</v>
       </c>
@@ -15259,7 +15383,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>70</v>
       </c>
@@ -15318,7 +15442,7 @@
         <v>6236</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>71</v>
       </c>
@@ -15377,7 +15501,7 @@
         <v>7466</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>72</v>
       </c>
@@ -15436,7 +15560,7 @@
         <v>7185</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>73</v>
       </c>
@@ -15495,7 +15619,7 @@
         <v>6327</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>74</v>
       </c>
@@ -15554,7 +15678,7 @@
         <v>7345</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>75</v>
       </c>
@@ -15613,7 +15737,7 @@
         <v>7471</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>76</v>
       </c>
@@ -15672,7 +15796,7 @@
         <v>6439</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>77</v>
       </c>
@@ -15731,47 +15855,47 @@
         <v>7307</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>86</v>
       </c>
@@ -15830,7 +15954,7 @@
         <v>7428</v>
       </c>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>87</v>
       </c>
@@ -15889,7 +16013,7 @@
         <v>7120</v>
       </c>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>88</v>
       </c>
@@ -15948,7 +16072,7 @@
         <v>7324</v>
       </c>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
         <v>89</v>
       </c>
@@ -16007,367 +16131,367 @@
         <v>9407</v>
       </c>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138" s="3" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146" s="3" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147" s="3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>48</v>
       </c>
@@ -16387,9 +16511,9 @@
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -16397,7 +16521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -16405,7 +16529,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -16413,7 +16537,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -16421,7 +16545,7 @@
         <v>45363</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -16429,7 +16553,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -16437,7 +16561,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -16445,7 +16569,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -16453,17 +16577,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -16471,7 +16595,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -16482,7 +16606,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -16493,7 +16617,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -16504,7 +16628,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -16515,7 +16639,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -16526,7 +16650,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -16534,7 +16658,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -16545,7 +16669,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -16556,7 +16680,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -16567,7 +16691,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -16578,7 +16702,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -16589,7 +16713,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -16597,12 +16721,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
@@ -16643,7 +16767,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>40</v>
       </c>
@@ -16684,7 +16808,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>41</v>
       </c>
@@ -16725,7 +16849,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>42</v>
       </c>
@@ -16766,7 +16890,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>43</v>
       </c>
@@ -16807,7 +16931,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>44</v>
       </c>
@@ -16848,7 +16972,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>45</v>
       </c>
@@ -16889,7 +17013,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>46</v>
       </c>
@@ -16930,7 +17054,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>47</v>
       </c>
@@ -16971,7 +17095,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -16991,9 +17115,9 @@
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -17001,7 +17125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -17009,7 +17133,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -17017,7 +17141,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -17025,7 +17149,7 @@
         <v>45363</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -17033,7 +17157,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -17041,7 +17165,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -17049,7 +17173,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -17057,17 +17181,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -17075,7 +17199,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -17086,7 +17210,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -17097,7 +17221,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -17108,7 +17232,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -17119,7 +17243,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -17130,7 +17254,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -17138,7 +17262,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -17149,7 +17273,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -17160,7 +17284,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -17171,7 +17295,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -17182,7 +17306,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -17193,7 +17317,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -17201,12 +17325,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
@@ -17247,7 +17371,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>40</v>
       </c>
@@ -17288,7 +17412,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>41</v>
       </c>
@@ -17329,7 +17453,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>42</v>
       </c>
@@ -17370,7 +17494,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>43</v>
       </c>
@@ -17411,7 +17535,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>44</v>
       </c>
@@ -17452,7 +17576,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>45</v>
       </c>
@@ -17493,7 +17617,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>46</v>
       </c>
@@ -17534,7 +17658,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>47</v>
       </c>
@@ -17575,7 +17699,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -17595,9 +17719,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -17605,7 +17729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -17613,7 +17737,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -17621,7 +17745,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -17629,7 +17753,7 @@
         <v>45363</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -17637,7 +17761,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -17645,7 +17769,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -17653,7 +17777,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -17661,17 +17785,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -17679,7 +17803,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -17690,7 +17814,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -17701,7 +17825,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -17712,7 +17836,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -17723,7 +17847,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -17734,7 +17858,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -17742,7 +17866,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -17753,7 +17877,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -17764,7 +17888,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -17775,7 +17899,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -17786,7 +17910,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -17797,7 +17921,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -17805,12 +17929,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
@@ -17851,7 +17975,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>40</v>
       </c>
@@ -17892,7 +18016,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>41</v>
       </c>
@@ -17933,7 +18057,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>42</v>
       </c>
@@ -17974,7 +18098,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>43</v>
       </c>
@@ -18015,7 +18139,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>44</v>
       </c>
@@ -18056,7 +18180,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>45</v>
       </c>
@@ -18097,7 +18221,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>46</v>
       </c>
@@ -18138,7 +18262,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>47</v>
       </c>
@@ -18179,7 +18303,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -18199,9 +18323,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>190</v>
       </c>

</xml_diff>